<commit_message>
Update TravisCI config and TCR import template
</commit_message>
<xml_diff>
--- a/tcrdb/resources/web/tcrdb/exampleData/ImportTemplate.xlsx
+++ b/tcrdb/resources/web/tcrdb/exampleData/ImportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\discvr18.2\externalModules\DISCVR\tcrdb\resources\web\tcrdb\exampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\discvr19.3\server\modules\BimberLabKeyModules\tcrdb\resources\web\tcrdb\exampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>HTO</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>TCR Library Conc</t>
-  </si>
-  <si>
-    <t>TCR Library Fragment Size</t>
-  </si>
-  <si>
-    <t>5' GEX Fragment Size</t>
   </si>
   <si>
     <t>Pool/Tube</t>
@@ -119,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -129,9 +123,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -431,114 +422,105 @@
     <col min="3" max="3" width="10.875" style="4"/>
     <col min="4" max="4" width="18.75" style="1" customWidth="1"/>
     <col min="5" max="10" width="10.875" style="1"/>
-    <col min="11" max="11" width="10.875" style="5"/>
-    <col min="12" max="12" width="12.25" style="1" customWidth="1"/>
-    <col min="13" max="14" width="10.875" style="1"/>
-    <col min="15" max="15" width="10.875" style="5"/>
-    <col min="16" max="16384" width="10.875" style="1"/>
+    <col min="11" max="11" width="12.25" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="P5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>